<commit_message>
modified as windows version
</commit_message>
<xml_diff>
--- a/database/Suggestion.xlsx
+++ b/database/Suggestion.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>铝</t>
   </si>
@@ -24,22 +23,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,26 +57,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -361,21 +373,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
@@ -383,11 +389,11 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>1.802451333813987</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upgrade the logic output with sf
</commit_message>
<xml_diff>
--- a/database/Suggestion.xlsx
+++ b/database/Suggestion.xlsx
@@ -14,9 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>现货变化</t>
+  </si>
+  <si>
+    <t>代码</t>
+  </si>
+  <si>
+    <t>期货价格</t>
+  </si>
+  <si>
+    <t>180极限</t>
+  </si>
+  <si>
+    <t>基差*极限</t>
+  </si>
   <si>
     <t>铝</t>
+  </si>
+  <si>
+    <t>1804</t>
   </si>
 </sst>
 </file>
@@ -374,23 +392,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1">
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1.802451333813987</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>14385</v>
+      </c>
+      <c r="E2">
+        <v>0.3868613138686132</v>
+      </c>
+      <c r="F2">
+        <v>-0.7260499162548335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>